<commit_message>
Correção das função de gerar relatorio, inicio relatorios personalizados
</commit_message>
<xml_diff>
--- a/RelatorioFaturamento.xlsx
+++ b/RelatorioFaturamento.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>Codigo Reserva</t>
   </si>
@@ -30,39 +30,6 @@
   </si>
   <si>
     <t>Valor Total Pago</t>
-  </si>
-  <si>
-    <t>2021-10-22T12:02:18-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-22T12:02:33-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-22T14:17:36-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-22T14:40:58-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-22T16:26:04-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-25T14:25:27-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-26T10:45:31-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-26T16:54:24-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-29T13:09:11-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-29T13:11:13-03:00</t>
-  </si>
-  <si>
-    <t>2021-10-29T13:11:18-03:00</t>
   </si>
 </sst>
 </file>
@@ -401,7 +368,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,193 +393,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>3.75</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>3.6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>3.6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>3.75</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>2.85</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>25.35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <v>2.55</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>8.6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>21</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>0.15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="D11">
-        <v>37.15</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>36.8</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>

<commit_message>
Correção do front Ende de index, redirecionamento de relatorios prontos para a função correta
</commit_message>
<xml_diff>
--- a/RelatorioFaturamento.xlsx
+++ b/RelatorioFaturamento.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Codigo Reserva</t>
   </si>
@@ -30,6 +30,39 @@
   </si>
   <si>
     <t>Valor Total Pago</t>
+  </si>
+  <si>
+    <t>2021-10-22T12:02:18-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-22T12:02:33-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-22T14:17:36-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-22T14:40:58-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-22T16:26:04-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-25T14:25:27-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-26T10:45:31-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-26T16:54:24-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T13:09:11-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T13:11:13-03:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T13:11:18-03:00</t>
   </si>
 </sst>
 </file>
@@ -368,7 +401,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -391,6 +424,193 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>25.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>2.55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>37.15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>36.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>